<commit_message>
Updated ITA model - 2025-08-16 11:07
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/source_data/VerveStacks_BGR.xlsx
+++ b/VerveStacks_BGR/source_data/VerveStacks_BGR.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE420B6-172E-4A28-B475-41BED6F546FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74F82C7-8A69-4CF7-A6E8-B5C830FD4772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="iamc_data" sheetId="73" r:id="rId1"/>
-    <sheet name="iamc_charts" sheetId="72" r:id="rId2"/>
-    <sheet name="weo_pg" sheetId="71" r:id="rId3"/>
-    <sheet name="re_targets" sheetId="70" r:id="rId4"/>
-    <sheet name="ccs_retrofits" sheetId="69" r:id="rId5"/>
-    <sheet name="Calibration" sheetId="68" r:id="rId6"/>
-    <sheet name="existing_stock" sheetId="67" r:id="rId7"/>
+    <sheet name="iamc_data" sheetId="80" r:id="rId1"/>
+    <sheet name="iamc_charts" sheetId="79" r:id="rId2"/>
+    <sheet name="weo_pg" sheetId="78" r:id="rId3"/>
+    <sheet name="re_targets" sheetId="77" r:id="rId4"/>
+    <sheet name="ccs_retrofits" sheetId="76" r:id="rId5"/>
+    <sheet name="Calibration" sheetId="75" r:id="rId6"/>
+    <sheet name="existing_stock" sheetId="74" r:id="rId7"/>
     <sheet name="historical_data_long" sheetId="5" r:id="rId8"/>
     <sheet name="historical_data" sheetId="4" r:id="rId9"/>
     <sheet name="system_settings" sheetId="1" r:id="rId10"/>
@@ -34,112 +34,7 @@
     <author>Amit Kanudia</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{6705E15F-52A0-4A16-9FD5-6A98D6455E38}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>💡 Three-letter ISO country code
-📊 CALCULATION: Direct from source data
-📁 DATA SOURCE: ISO 3166-1 alpha-3 standard
-🔧 METHODOLOGY: Standardized country identification
-✅ QUALITY: Verified against official ISO registry
-→ See row 4 for complete methodology</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{80150844-B1F9-40D9-9CCE-56FDEB6B1488}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>💡 Standardized fuel/technology category
-📊 CALCULATION: Mapped from source technology classifications
-📁 DATA SOURCE: GEM/IRENA/EMBER technology categories
-🔧 METHODOLOGY: Harmonized technology mapping across all sources
-✅ QUALITY: Consistent categorization ensures comparability
-→ See row 4 for complete methodology</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{82ABAAA5-D6C4-413A-B1CE-5827CCBBCA45}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>💡 Installed capacity from Global Energy Monitor
-📊 CALCULATION: Sum of individual plant capacities by technology
-📁 DATA SOURCE: GEM Global Power Plant Tracker
-🔧 METHODOLOGY: Facility-level data aggregated by fuel type
-✅ QUALITY: Most granular source with individual plant details
-→ See row 4 for complete methodology</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{78515C2B-5B41-4507-92DF-51CEF6F402A8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>💡 Installed capacity from IRENA statistics
-📊 CALCULATION: National statistics by technology category
-📁 DATA SOURCE: IRENA Renewable Energy Statistics
-🔧 METHODOLOGY: Official government reporting aggregated by IRENA
-✅ QUALITY: Authoritative for renewables, may include distributed generation
-→ See row 4 for complete methodology</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00C261AA-19F8-45A4-B3FD-9DFF6A427FC7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>💡 Installed capacity from Ember statistics
-📊 CALCULATION: National statistics by technology category
-📁 DATA SOURCE: Ember Global Electricity Review
-🔧 METHODOLOGY: Statistical analysis of electricity sector data
-✅ QUALITY: Focus on electricity sector, excludes some industrial capacity
-→ See row 4 for complete methodology</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Amit Kanudia</author>
-  </authors>
-  <commentList>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{7048D575-D9A3-413B-A0E6-484216D28FE4}">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{14D2474C-0145-49F9-BCDD-6EA1FD5BC86F}">
       <text>
         <r>
           <rPr>
@@ -158,7 +53,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{60846A03-CAC0-4D5B-88DD-6FEA0573C83F}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{BB38EFF4-D337-4C3C-BEE6-9F1033171677}">
       <text>
         <r>
           <rPr>
@@ -177,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{EA13D1FC-B224-473D-85CE-EFC7B10F4306}">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{E8C4748B-F58E-4349-996A-13C4E7691F5C}">
       <text>
         <r>
           <rPr>
@@ -196,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{78F9E225-C70D-4084-BE56-CEC2FC89A0A5}">
+    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{4B640805-4C4A-4670-B1FA-8A2B94BB440C}">
       <text>
         <r>
           <rPr>
@@ -215,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{A8A96C4B-C3A8-4312-A5D0-5852ECC2CED0}">
+    <comment ref="M6" authorId="0" shapeId="0" xr:uid="{0743E34E-BD20-444C-802D-7693347B5663}">
       <text>
         <r>
           <rPr>
@@ -234,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{CD63214C-6711-447F-8D10-856F48D8C21A}">
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{0C081194-44F7-45BA-A11C-D2C6CF480B3E}">
       <text>
         <r>
           <rPr>
@@ -253,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{385C3DAD-616F-47ED-9956-EE671891E332}">
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{F67CF14F-E95F-42E4-9F0D-07F28DF3A866}">
       <text>
         <r>
           <rPr>
@@ -276,7 +171,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Amit Kanudia</author>
@@ -304,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8736" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8733" uniqueCount="401">
   <si>
     <t>Time Slices</t>
   </si>
@@ -1516,22 +1411,13 @@
 </t>
   </si>
   <si>
-    <t>Table 1: Installed Capacity Comparison (GW)</t>
-  </si>
-  <si>
-    <t>calibration_capacity</t>
-  </si>
-  <si>
     <t>Table 2: Generation Analysis (TWh)</t>
-  </si>
-  <si>
-    <t>calibration_generation</t>
   </si>
   <si>
     <t>Table 3: Detailed Metrics &amp; Validation</t>
   </si>
   <si>
-    <t>calibration_analysis</t>
+    <t>Table 1: Capacity Comparison (GW)</t>
   </si>
 </sst>
 </file>
@@ -1544,7 +1430,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1609,16 +1495,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1640,6 +1518,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF7F9FC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF0F8FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1686,7 +1570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1702,7 +1586,6 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="167" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1710,13 +1593,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1759,7 +1642,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FED7B2F-9974-47C5-A93B-FE7DF48B1AE8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DB908F9-9827-425B-3B65-742F7A9ACE82}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1814,7 +1697,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E48E0751-F35B-E442-F5F5-5B15BCF62A95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD3D33C-B18A-6265-A4EF-69BB68BF7F4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1869,7 +1752,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C4976A7-D86B-3CD7-2A4D-DA16AEC982EF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097E44CD-4AA0-AF92-75BC-8DB0538720D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1924,7 +1807,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A11AC5F-22BF-4144-03D8-9F8075E1779C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4295E313-B9EF-3065-745A-7650E5E4DFCE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1979,7 +1862,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F93D73FF-0196-7187-71B8-0ADEA2B0FE08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CACB5D0F-D623-8596-6CF0-C19325C61078}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2034,7 +1917,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0CE8627-D7A7-53F1-7B1A-7412A71B932B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC98DB86-FD70-7047-53C6-58E9C5A1C301}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2571,6 +2454,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>296863</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{088654C1-45A0-6F86-6FAC-EFAFC6B134CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17479963" y="12700"/>
+          <a:ext cx="990600" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2890,7 +2823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D460486-16B9-416D-A774-93682F7286B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B752AA81-2F31-413C-BFAD-255BBE959670}">
   <dimension ref="A1:L638"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -25656,7 +25589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32DDF671-E877-4C61-BE69-98C34EB2EE11}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DB85094-C4B3-41DD-A2D1-3FCC7EC58A91}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -25669,7 +25602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB5F688-EBFC-4887-90C5-502147C8F2F8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392E1D91-98D4-4969-A3B2-5884029CB337}">
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25687,16 +25620,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
@@ -28889,7 +28822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4DD3E8-036B-4D45-B8C9-9FA4701BE14C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D7B59D-B3EC-4F80-9EEA-44CBE2F4A94B}">
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28909,17 +28842,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
@@ -28983,7 +28916,7 @@
       <c r="H4" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="17">
         <v>45343</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -29018,7 +28951,7 @@
       <c r="H5" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>44949</v>
       </c>
       <c r="J5" s="9" t="s">
@@ -29053,7 +28986,7 @@
       <c r="H6" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="17">
         <v>44949</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -29088,7 +29021,7 @@
       <c r="H7" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="18">
         <v>45343</v>
       </c>
       <c r="J7" s="9" t="s">
@@ -29123,7 +29056,7 @@
       <c r="H8" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="17">
         <v>44949</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -29158,7 +29091,7 @@
       <c r="H9" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="18">
         <v>45343</v>
       </c>
       <c r="J9" s="9" t="s">
@@ -29193,7 +29126,7 @@
       <c r="H10" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="17">
         <v>44949</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -29228,7 +29161,7 @@
       <c r="H11" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="18">
         <v>44949</v>
       </c>
       <c r="J11" s="9" t="s">
@@ -29263,7 +29196,7 @@
       <c r="H12" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="17">
         <v>45343</v>
       </c>
       <c r="J12" s="4" t="s">
@@ -29298,7 +29231,7 @@
       <c r="H13" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="18">
         <v>44949</v>
       </c>
       <c r="J13" s="9" t="s">
@@ -29333,7 +29266,7 @@
       <c r="H14" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="17">
         <v>45343</v>
       </c>
       <c r="J14" s="4" t="s">
@@ -29368,7 +29301,7 @@
       <c r="H15" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="18">
         <v>45343</v>
       </c>
       <c r="J15" s="9" t="s">
@@ -29403,7 +29336,7 @@
       <c r="H16" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="17">
         <v>45343</v>
       </c>
       <c r="J16" s="4" t="s">
@@ -29438,7 +29371,7 @@
       <c r="H17" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="18">
         <v>45343</v>
       </c>
       <c r="J17" s="9" t="s">
@@ -29473,7 +29406,7 @@
       <c r="H18" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="17">
         <v>45343</v>
       </c>
       <c r="J18" s="4" t="s">
@@ -29508,7 +29441,7 @@
       <c r="H19" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="I19" s="19">
+      <c r="I19" s="18">
         <v>45343</v>
       </c>
       <c r="J19" s="9" t="s">
@@ -29543,7 +29476,7 @@
       <c r="H20" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="17">
         <v>45343</v>
       </c>
       <c r="J20" s="4" t="s">
@@ -29566,7 +29499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6025E80C-DFD4-48E4-804D-579844FE5DA8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFF9BFC-582E-47CF-A041-2254B3BA892D}">
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -29583,16 +29516,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="2" t="s">
@@ -30508,8 +30441,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9EC6EA-F3D7-44CF-B0FC-0D99A2B915E3}">
-  <dimension ref="A1:J41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845885DD-2311-4D11-90D9-243F08628A97}">
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -30527,70 +30460,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="15" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A8" s="14" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C6" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D6" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E6" s="3" t="s">
         <v>383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13">
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
@@ -30598,16 +30558,14 @@
         <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="C9" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.1</v>
-      </c>
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="8"/>
       <c r="E9" s="8">
-        <v>0.1</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
@@ -30615,14 +30573,16 @@
         <v>52</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="C10" s="13">
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="D10" s="13"/>
+        <v>3.3</v>
+      </c>
+      <c r="D10" s="13">
+        <v>3.3</v>
+      </c>
       <c r="E10" s="13">
-        <v>5.0999999999999996</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
@@ -30630,14 +30590,16 @@
         <v>52</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="C11" s="8">
-        <v>1.2</v>
-      </c>
-      <c r="D11" s="8"/>
+        <v>2.1</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2</v>
+      </c>
       <c r="E11" s="8">
-        <v>1.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
@@ -30645,16 +30607,16 @@
         <v>52</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="C12" s="13">
-        <v>3.3</v>
+        <v>1.7</v>
       </c>
       <c r="D12" s="13">
-        <v>3.3</v>
+        <v>1.7</v>
       </c>
       <c r="E12" s="13">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
@@ -30662,415 +30624,371 @@
         <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12">
+        <v>21.8</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7">
+        <v>2.1</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="12">
+        <v>3.8</v>
+      </c>
+      <c r="D21" s="12">
+        <v>5</v>
+      </c>
+      <c r="E21" s="12">
+        <v>3.8</v>
+      </c>
+      <c r="F21" s="12">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C22" s="7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="D22" s="7">
+        <v>17</v>
+      </c>
+      <c r="E22" s="7">
+        <v>16.5</v>
+      </c>
+      <c r="F22" s="7">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C23" s="12">
         <v>2.1</v>
       </c>
-      <c r="D13" s="8">
-        <v>2</v>
-      </c>
-      <c r="E13" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="D23" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="E23" s="12">
+        <v>2.1</v>
+      </c>
+      <c r="F23" s="12">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="8">
+        <v>3.25</v>
+      </c>
+      <c r="D29" s="8">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="F29" s="7">
+        <v>4.3</v>
+      </c>
+      <c r="G29" s="7">
+        <v>6.8</v>
+      </c>
+      <c r="H29" s="7">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13">
+        <v>0.49</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.33</v>
+      </c>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12">
+        <v>66</v>
+      </c>
+      <c r="H30" s="12">
+        <v>110.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7">
+        <v>5.9</v>
+      </c>
+      <c r="H31" s="7">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="13">
+        <v>0.13</v>
+      </c>
+      <c r="D32" s="13">
+        <v>0.17</v>
+      </c>
+      <c r="E32" s="13">
+        <v>1</v>
+      </c>
+      <c r="F32" s="12">
+        <v>3.8</v>
+      </c>
+      <c r="G32" s="12">
+        <v>5</v>
+      </c>
+      <c r="H32" s="12"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="8">
+        <v>0.94</v>
+      </c>
+      <c r="D33" s="8">
+        <v>0.93</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1</v>
+      </c>
+      <c r="F33" s="7">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="G33" s="7">
+        <v>17</v>
+      </c>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A34" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="C14" s="13">
-        <v>1.7</v>
-      </c>
-      <c r="D14" s="13">
-        <v>1.7</v>
-      </c>
-      <c r="E14" s="13">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="15" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="2" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="D22" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E22" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F22" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12">
-        <v>21.8</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12">
-        <v>21.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7">
+      <c r="C34" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D34" s="13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E34" s="13">
+        <v>1</v>
+      </c>
+      <c r="F34" s="12">
         <v>2.1</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7">
+      <c r="G34" s="12">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C25" s="12">
-        <v>3.8</v>
-      </c>
-      <c r="D25" s="12">
-        <v>5</v>
-      </c>
-      <c r="E25" s="12">
-        <v>3.8</v>
-      </c>
-      <c r="F25" s="12">
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C26" s="7">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="D26" s="7">
-        <v>17</v>
-      </c>
-      <c r="E26" s="7">
-        <v>16.5</v>
-      </c>
-      <c r="F26" s="7">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A27" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C27" s="12">
-        <v>2.1</v>
-      </c>
-      <c r="D27" s="12">
-        <v>2.1</v>
-      </c>
-      <c r="E27" s="12">
-        <v>2.1</v>
-      </c>
-      <c r="F27" s="12">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C28" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="D28" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="E28" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="F28" s="7">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A32" s="15" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A34" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>393</v>
-      </c>
+      <c r="H34" s="12"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>79</v>
+        <v>209</v>
       </c>
       <c r="C35" s="8">
-        <v>3.25</v>
+        <v>0.24</v>
       </c>
       <c r="D35" s="8">
-        <v>5.1100000000000003</v>
+        <v>0.23</v>
       </c>
       <c r="E35" s="8">
-        <v>0.33</v>
+        <v>1</v>
       </c>
       <c r="F35" s="7">
-        <v>4.3</v>
+        <v>1.5</v>
       </c>
       <c r="G35" s="7">
-        <v>6.8</v>
-      </c>
-      <c r="H35" s="7">
-        <v>7.6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13">
-        <v>0.49</v>
-      </c>
-      <c r="E36" s="13">
-        <v>0.33</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12">
-        <v>66</v>
-      </c>
-      <c r="H36" s="12">
-        <v>110.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="E37" s="8">
-        <v>0.36</v>
-      </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7">
-        <v>5.9</v>
-      </c>
-      <c r="H37" s="7">
-        <v>10.3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="13">
-        <v>0.13</v>
-      </c>
-      <c r="D38" s="13">
-        <v>0.17</v>
-      </c>
-      <c r="E38" s="13">
-        <v>1</v>
-      </c>
-      <c r="F38" s="12">
-        <v>3.8</v>
-      </c>
-      <c r="G38" s="12">
-        <v>5</v>
-      </c>
-      <c r="H38" s="12"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C39" s="8">
-        <v>0.94</v>
-      </c>
-      <c r="D39" s="8">
-        <v>0.93</v>
-      </c>
-      <c r="E39" s="8">
-        <v>1</v>
-      </c>
-      <c r="F39" s="7">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="G39" s="7">
-        <v>17</v>
-      </c>
-      <c r="H39" s="7"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="C40" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D40" s="13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E40" s="13">
-        <v>1</v>
-      </c>
-      <c r="F40" s="12">
-        <v>2.1</v>
-      </c>
-      <c r="G40" s="12">
-        <v>2.1</v>
-      </c>
-      <c r="H40" s="12"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C41" s="8">
-        <v>0.24</v>
-      </c>
-      <c r="D41" s="8">
-        <v>0.23</v>
-      </c>
-      <c r="E41" s="8">
-        <v>1</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="G41" s="7">
         <v>1.4</v>
       </c>
-      <c r="H41" s="7"/>
+      <c r="H35" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -31080,12 +30998,11 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA87927B-DE2E-4A38-B100-E3F22D8920E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23354DE-66D9-4D8F-988B-DC2ABB584402}">
   <dimension ref="A1:W91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -31114,57 +31031,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>394</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>395</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
     </row>
     <row r="5" spans="1:23" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
@@ -46020,31 +45937,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
     </row>
     <row r="2" spans="1:25" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
@@ -49402,76 +49319,76 @@
       <c r="A57" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B57" s="16">
+      <c r="B57" s="15">
         <v>0</v>
       </c>
-      <c r="C57" s="16">
+      <c r="C57" s="15">
         <v>0</v>
       </c>
-      <c r="D57" s="16">
+      <c r="D57" s="15">
         <v>0</v>
       </c>
-      <c r="E57" s="16">
+      <c r="E57" s="15">
         <v>0</v>
       </c>
-      <c r="F57" s="16">
+      <c r="F57" s="15">
         <v>0</v>
       </c>
-      <c r="G57" s="16">
+      <c r="G57" s="15">
         <v>0</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="15">
         <v>0</v>
       </c>
-      <c r="I57" s="16">
+      <c r="I57" s="15">
         <v>0</v>
       </c>
-      <c r="J57" s="16">
+      <c r="J57" s="15">
         <v>0.22831050228310504</v>
       </c>
-      <c r="K57" s="16">
+      <c r="K57" s="15">
         <v>0.11415525114155252</v>
       </c>
-      <c r="L57" s="16">
+      <c r="L57" s="15">
         <v>0.45662100456621008</v>
       </c>
-      <c r="M57" s="16">
+      <c r="M57" s="15">
         <v>0.68493150684931503</v>
       </c>
-      <c r="N57" s="16">
+      <c r="N57" s="15">
         <v>0.7990867579908677</v>
       </c>
-      <c r="O57" s="16">
+      <c r="O57" s="15">
         <v>0.41856925418569257</v>
       </c>
-      <c r="P57" s="16">
+      <c r="P57" s="15">
         <v>0.57077625570776258</v>
       </c>
-      <c r="Q57" s="16">
+      <c r="Q57" s="15">
         <v>0.61643835616438358</v>
       </c>
-      <c r="R57" s="16">
+      <c r="R57" s="15">
         <v>0.66590563165905636</v>
       </c>
-      <c r="S57" s="16">
+      <c r="S57" s="15">
         <v>0.91324200913242015</v>
       </c>
-      <c r="T57" s="16">
+      <c r="T57" s="15">
         <v>2.5603392041748205</v>
       </c>
-      <c r="U57" s="16">
+      <c r="U57" s="15">
         <v>3.4627092846270933</v>
       </c>
-      <c r="V57" s="16">
+      <c r="V57" s="15">
         <v>3.8812785388127851</v>
       </c>
-      <c r="W57" s="16">
+      <c r="W57" s="15">
         <v>5.9132420091324196</v>
       </c>
-      <c r="X57" s="16">
+      <c r="X57" s="15">
         <v>5.1141552511415531</v>
       </c>
-      <c r="Y57" s="16">
+      <c r="Y57" s="15">
         <v>4.9771689497716896</v>
       </c>
     </row>
@@ -49479,76 +49396,76 @@
       <c r="A58" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B58" s="17">
+      <c r="B58" s="16">
         <v>0.34409073920603195</v>
       </c>
-      <c r="C58" s="17">
+      <c r="C58" s="16">
         <v>0.39609028421001313</v>
       </c>
-      <c r="D58" s="17">
+      <c r="D58" s="16">
         <v>0.34896569655015519</v>
       </c>
-      <c r="E58" s="17">
+      <c r="E58" s="16">
         <v>0.3908090804205463</v>
       </c>
-      <c r="F58" s="17">
+      <c r="F58" s="16">
         <v>0.3922789539227895</v>
       </c>
-      <c r="G58" s="17">
+      <c r="G58" s="16">
         <v>0.38314653383146535</v>
       </c>
-      <c r="H58" s="17">
+      <c r="H58" s="16">
         <v>0.396222498962225</v>
       </c>
-      <c r="I58" s="17">
+      <c r="I58" s="16">
         <v>0.46430053964300544</v>
       </c>
-      <c r="J58" s="17">
+      <c r="J58" s="16">
         <v>0.48111249481112495</v>
       </c>
-      <c r="K58" s="17">
+      <c r="K58" s="16">
         <v>0.42782873873654675</v>
       </c>
-      <c r="L58" s="17">
+      <c r="L58" s="16">
         <v>0.45844586648499153</v>
       </c>
-      <c r="M58" s="17">
+      <c r="M58" s="16">
         <v>0.49726171897578175</v>
       </c>
-      <c r="N58" s="17">
+      <c r="N58" s="16">
         <v>0.41309028379862439</v>
       </c>
-      <c r="O58" s="17">
+      <c r="O58" s="16">
         <v>0.36227010141320837</v>
       </c>
-      <c r="P58" s="17">
+      <c r="P58" s="16">
         <v>0.41231328844516674</v>
       </c>
-      <c r="Q58" s="17">
+      <c r="Q58" s="16">
         <v>0.50828415182197206</v>
       </c>
-      <c r="R58" s="17">
+      <c r="R58" s="16">
         <v>0.4369935206742831</v>
       </c>
-      <c r="S58" s="17">
+      <c r="S58" s="16">
         <v>0.46734400271649285</v>
       </c>
-      <c r="T58" s="17">
+      <c r="T58" s="16">
         <v>0.41685655309224456</v>
       </c>
-      <c r="U58" s="17">
+      <c r="U58" s="16">
         <v>0.38424076705180099</v>
       </c>
-      <c r="V58" s="17">
+      <c r="V58" s="16">
         <v>0.30180771877150181</v>
       </c>
-      <c r="W58" s="17">
+      <c r="W58" s="16">
         <v>0.38178341330902782</v>
       </c>
-      <c r="X58" s="17">
+      <c r="X58" s="16">
         <v>0.48677943686388042</v>
       </c>
-      <c r="Y58" s="17">
+      <c r="Y58" s="16">
         <v>0.25824553878597789</v>
       </c>
     </row>
@@ -49556,76 +49473,76 @@
       <c r="A59" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="15">
         <v>0.19642930601834707</v>
       </c>
-      <c r="C59" s="16">
+      <c r="C59" s="15">
         <v>0.19642930601834707</v>
       </c>
-      <c r="D59" s="16">
+      <c r="D59" s="15">
         <v>0.1583775556378296</v>
       </c>
-      <c r="E59" s="16">
+      <c r="E59" s="15">
         <v>0.18100292072894811</v>
       </c>
-      <c r="F59" s="16">
+      <c r="F59" s="15">
         <v>0.15323542720802993</v>
       </c>
-      <c r="G59" s="16">
+      <c r="G59" s="15">
         <v>0.1779176436710683</v>
       </c>
-      <c r="H59" s="16">
+      <c r="H59" s="15">
         <v>0.22213994816734542</v>
       </c>
-      <c r="I59" s="16">
+      <c r="I59" s="15">
         <v>0.23228111971411552</v>
       </c>
-      <c r="J59" s="16">
+      <c r="J59" s="15">
         <v>0.23426642842962081</v>
       </c>
-      <c r="K59" s="16">
+      <c r="K59" s="15">
         <v>0.19456025411951558</v>
       </c>
-      <c r="L59" s="16">
+      <c r="L59" s="15">
         <v>0.19555290847726822</v>
       </c>
-      <c r="M59" s="16">
+      <c r="M59" s="15">
         <v>0.19786910197869106</v>
       </c>
-      <c r="N59" s="16">
+      <c r="N59" s="15">
         <v>0.22450532724505329</v>
       </c>
-      <c r="O59" s="16">
+      <c r="O59" s="15">
         <v>0.2226027397260274</v>
       </c>
-      <c r="P59" s="16">
+      <c r="P59" s="15">
         <v>0.20357686453576868</v>
       </c>
-      <c r="Q59" s="16">
+      <c r="Q59" s="15">
         <v>0.17694063926940642</v>
       </c>
-      <c r="R59" s="16">
+      <c r="R59" s="15">
         <v>0.1950152207001522</v>
       </c>
-      <c r="S59" s="16">
+      <c r="S59" s="15">
         <v>0.18359969558599698</v>
       </c>
-      <c r="T59" s="16">
+      <c r="T59" s="15">
         <v>0.19216133942161343</v>
       </c>
-      <c r="U59" s="16">
+      <c r="U59" s="15">
         <v>0.20452815829528159</v>
       </c>
-      <c r="V59" s="16">
+      <c r="V59" s="15">
         <v>0.21784627092846273</v>
       </c>
-      <c r="W59" s="16">
+      <c r="W59" s="15">
         <v>0.29014459665144599</v>
       </c>
-      <c r="X59" s="16">
+      <c r="X59" s="15">
         <v>0.1950152207001522</v>
       </c>
-      <c r="Y59" s="16">
+      <c r="Y59" s="15">
         <v>0.14840182648401828</v>
       </c>
     </row>
@@ -49633,76 +49550,76 @@
       <c r="A60" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B60" s="17">
+      <c r="B60" s="16">
         <v>0.29434148088459128</v>
       </c>
-      <c r="C60" s="17">
+      <c r="C60" s="16">
         <v>0.22423352902804958</v>
       </c>
-      <c r="D60" s="17">
+      <c r="D60" s="16">
         <v>0.22408253001860307</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="16">
         <v>0.20686315206863154</v>
       </c>
-      <c r="F60" s="17">
+      <c r="F60" s="16">
         <v>0.18103408514367419</v>
       </c>
-      <c r="G60" s="17">
+      <c r="G60" s="16">
         <v>0.24791291914579586</v>
       </c>
-      <c r="H60" s="17">
+      <c r="H60" s="16">
         <v>0.2427240440939071</v>
       </c>
-      <c r="I60" s="17">
+      <c r="I60" s="16">
         <v>0.16072605011472321</v>
       </c>
-      <c r="J60" s="17">
+      <c r="J60" s="16">
         <v>0.1502326182476092</v>
       </c>
-      <c r="K60" s="17">
+      <c r="K60" s="16">
         <v>0.18296846327828276</v>
       </c>
-      <c r="L60" s="17">
+      <c r="L60" s="16">
         <v>0.26339491433119683</v>
       </c>
-      <c r="M60" s="17">
+      <c r="M60" s="16">
         <v>0.14626141552511415</v>
       </c>
-      <c r="N60" s="17">
+      <c r="N60" s="16">
         <v>0.15647142182333496</v>
       </c>
-      <c r="O60" s="17">
+      <c r="O60" s="16">
         <v>0.19708855325293684</v>
       </c>
-      <c r="P60" s="17">
+      <c r="P60" s="16">
         <v>0.22250599798777185</v>
       </c>
-      <c r="Q60" s="17">
+      <c r="Q60" s="16">
         <v>0.27329541057193724</v>
       </c>
-      <c r="R60" s="17">
+      <c r="R60" s="16">
         <v>0.18767897221577279</v>
       </c>
-      <c r="S60" s="17">
+      <c r="S60" s="16">
         <v>0.12870890865760704</v>
       </c>
-      <c r="T60" s="17">
+      <c r="T60" s="16">
         <v>0.23422292564900221</v>
       </c>
-      <c r="U60" s="17">
+      <c r="U60" s="16">
         <v>0.13325692663137406</v>
       </c>
-      <c r="V60" s="17">
+      <c r="V60" s="16">
         <v>0.12825410686023031</v>
       </c>
-      <c r="W60" s="17">
+      <c r="W60" s="16">
         <v>0.21921446633557101</v>
       </c>
-      <c r="X60" s="17">
+      <c r="X60" s="16">
         <v>0.17145847997545438</v>
       </c>
-      <c r="Y60" s="17">
+      <c r="Y60" s="16">
         <v>0.14032522966412186</v>
       </c>
     </row>
@@ -49710,76 +49627,76 @@
       <c r="A61" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B61" s="16">
+      <c r="B61" s="15">
         <v>0.58791571267802401</v>
       </c>
-      <c r="C61" s="16">
+      <c r="C61" s="15">
         <v>0.632219592016247</v>
       </c>
-      <c r="D61" s="16">
+      <c r="D61" s="15">
         <v>0.84860999194198217</v>
       </c>
-      <c r="E61" s="16">
+      <c r="E61" s="15">
         <v>0.72522159548751008</v>
       </c>
-      <c r="F61" s="16">
+      <c r="F61" s="15">
         <v>0.70591592801504166</v>
       </c>
-      <c r="G61" s="16">
+      <c r="G61" s="15">
         <v>0.78271890948160072</v>
       </c>
-      <c r="H61" s="16">
+      <c r="H61" s="15">
         <v>0.81797273704002138</v>
       </c>
-      <c r="I61" s="16">
+      <c r="I61" s="15">
         <v>0.88425019931869253</v>
       </c>
-      <c r="J61" s="16">
+      <c r="J61" s="15">
         <v>0.95250175158850958</v>
       </c>
-      <c r="K61" s="16">
+      <c r="K61" s="15">
         <v>0.92169795366142393</v>
       </c>
-      <c r="L61" s="16">
+      <c r="L61" s="15">
         <v>0.92109395762363799</v>
       </c>
-      <c r="M61" s="16">
+      <c r="M61" s="15">
         <v>0.98511753762895304</v>
       </c>
-      <c r="N61" s="16">
+      <c r="N61" s="15">
         <v>0.94312558272968505</v>
       </c>
-      <c r="O61" s="16">
+      <c r="O61" s="15">
         <v>0.81695954983626218</v>
       </c>
-      <c r="P61" s="16">
+      <c r="P61" s="15">
         <v>0.91497163414971638</v>
       </c>
-      <c r="Q61" s="16">
+      <c r="Q61" s="15">
         <v>0.88672109220054429</v>
       </c>
-      <c r="R61" s="16">
+      <c r="R61" s="15">
         <v>0.91440094569223274</v>
       </c>
-      <c r="S61" s="16">
+      <c r="S61" s="15">
         <v>0.90107317525438657</v>
       </c>
-      <c r="T61" s="16">
+      <c r="T61" s="15">
         <v>0.91608169199663791</v>
       </c>
-      <c r="U61" s="16">
+      <c r="U61" s="15">
         <v>0.94050296462891025</v>
       </c>
-      <c r="V61" s="16">
+      <c r="V61" s="15">
         <v>0.9444785206388151</v>
       </c>
-      <c r="W61" s="16">
+      <c r="W61" s="15">
         <v>0.93652740861900541</v>
       </c>
-      <c r="X61" s="16">
+      <c r="X61" s="15">
         <v>0.93482359890047495</v>
       </c>
-      <c r="Y61" s="16">
+      <c r="Y61" s="15">
         <v>0.91778550171516859</v>
       </c>
     </row>
@@ -49787,76 +49704,76 @@
       <c r="A62" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="B62" s="17">
+      <c r="B62" s="16">
         <v>65535</v>
       </c>
-      <c r="C62" s="17">
+      <c r="C62" s="16">
         <v>65535</v>
       </c>
-      <c r="D62" s="17">
+      <c r="D62" s="16">
         <v>65535</v>
       </c>
-      <c r="E62" s="17">
+      <c r="E62" s="16">
         <v>65535</v>
       </c>
-      <c r="F62" s="17">
+      <c r="F62" s="16">
         <v>65535</v>
       </c>
-      <c r="G62" s="17">
+      <c r="G62" s="16">
         <v>65535</v>
       </c>
-      <c r="H62" s="17">
+      <c r="H62" s="16">
         <v>65535</v>
       </c>
-      <c r="I62" s="17">
+      <c r="I62" s="16">
         <v>65535</v>
       </c>
-      <c r="J62" s="17">
+      <c r="J62" s="16">
         <v>65535</v>
       </c>
-      <c r="K62" s="17">
+      <c r="K62" s="16">
         <v>65535</v>
       </c>
-      <c r="L62" s="17">
+      <c r="L62" s="16">
         <v>65535</v>
       </c>
-      <c r="M62" s="17">
+      <c r="M62" s="16">
         <v>65535</v>
       </c>
-      <c r="N62" s="17">
+      <c r="N62" s="16">
         <v>65535</v>
       </c>
-      <c r="O62" s="17">
+      <c r="O62" s="16">
         <v>65535</v>
       </c>
-      <c r="P62" s="17">
+      <c r="P62" s="16">
         <v>65535</v>
       </c>
-      <c r="Q62" s="17">
+      <c r="Q62" s="16">
         <v>65535</v>
       </c>
-      <c r="R62" s="17">
+      <c r="R62" s="16">
         <v>65535</v>
       </c>
-      <c r="S62" s="17">
+      <c r="S62" s="16">
         <v>65535</v>
       </c>
-      <c r="T62" s="17">
+      <c r="T62" s="16">
         <v>65535</v>
       </c>
-      <c r="U62" s="17">
+      <c r="U62" s="16">
         <v>65535</v>
       </c>
-      <c r="V62" s="17">
+      <c r="V62" s="16">
         <v>65535</v>
       </c>
-      <c r="W62" s="17">
+      <c r="W62" s="16">
         <v>65535</v>
       </c>
-      <c r="X62" s="17">
+      <c r="X62" s="16">
         <v>65535</v>
       </c>
-      <c r="Y62" s="17">
+      <c r="Y62" s="16">
         <v>65535</v>
       </c>
     </row>
@@ -49864,56 +49781,56 @@
       <c r="A63" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="16"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="16">
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15">
         <v>3.8051750380517509E-2</v>
       </c>
-      <c r="M63" s="16">
+      <c r="M63" s="15">
         <v>7.6103500761035017E-2</v>
       </c>
-      <c r="N63" s="16">
+      <c r="N63" s="15">
         <v>9.6783799880881469E-2</v>
       </c>
-      <c r="O63" s="16">
+      <c r="O63" s="15">
         <v>0.1525728837372673</v>
       </c>
-      <c r="P63" s="16">
+      <c r="P63" s="15">
         <v>0.13964622955180209</v>
       </c>
-      <c r="Q63" s="16">
+      <c r="Q63" s="15">
         <v>0.15294587046149752</v>
       </c>
-      <c r="R63" s="16">
+      <c r="R63" s="15">
         <v>0.1540541738706388</v>
       </c>
-      <c r="S63" s="16">
+      <c r="S63" s="15">
         <v>0.15516247727978011</v>
       </c>
-      <c r="T63" s="16">
+      <c r="T63" s="15">
         <v>0.14851265682493239</v>
       </c>
-      <c r="U63" s="16">
+      <c r="U63" s="15">
         <v>0.15586582367404284</v>
       </c>
-      <c r="V63" s="16">
+      <c r="V63" s="15">
         <v>0.15255292652552924</v>
       </c>
-      <c r="W63" s="16">
+      <c r="W63" s="15">
         <v>0.13213245604573401</v>
       </c>
-      <c r="X63" s="16">
+      <c r="X63" s="15">
         <v>0.13711751430220961</v>
       </c>
-      <c r="Y63" s="16">
+      <c r="Y63" s="15">
         <v>0.13667567483614451</v>
       </c>
     </row>
@@ -49921,66 +49838,66 @@
       <c r="A64" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="17"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="17">
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16">
         <v>0</v>
       </c>
-      <c r="H64" s="17">
+      <c r="H64" s="16">
         <v>7.6103500761035017E-2</v>
       </c>
-      <c r="I64" s="17">
+      <c r="I64" s="16">
         <v>0.19025875190258754</v>
       </c>
-      <c r="J64" s="17">
+      <c r="J64" s="16">
         <v>0.12453300124533001</v>
       </c>
-      <c r="K64" s="17">
+      <c r="K64" s="16">
         <v>8.3022000830220002E-2</v>
       </c>
-      <c r="L64" s="17">
+      <c r="L64" s="16">
         <v>0.15841953219644023</v>
       </c>
-      <c r="M64" s="17">
+      <c r="M64" s="16">
         <v>0.18180280737358362</v>
       </c>
-      <c r="N64" s="17">
+      <c r="N64" s="16">
         <v>0.20480795057749127</v>
       </c>
-      <c r="O64" s="17">
+      <c r="O64" s="16">
         <v>0.22998925597636316</v>
       </c>
-      <c r="P64" s="17">
+      <c r="P64" s="16">
         <v>0.21689497716894979</v>
       </c>
-      <c r="Q64" s="17">
+      <c r="Q64" s="16">
         <v>0.23646444879321593</v>
       </c>
-      <c r="R64" s="17">
+      <c r="R64" s="16">
         <v>0.23157208088714937</v>
       </c>
-      <c r="S64" s="17">
+      <c r="S64" s="16">
         <v>0.24461839530332682</v>
       </c>
-      <c r="T64" s="17">
+      <c r="T64" s="16">
         <v>0.21526418786692761</v>
       </c>
-      <c r="U64" s="17">
+      <c r="U64" s="16">
         <v>0.21526418786692761</v>
       </c>
-      <c r="V64" s="17">
+      <c r="V64" s="16">
         <v>0.24135681669928247</v>
       </c>
-      <c r="W64" s="17">
+      <c r="W64" s="16">
         <v>0.23320287018917157</v>
       </c>
-      <c r="X64" s="17">
+      <c r="X64" s="16">
         <v>0.23483365949119375</v>
       </c>
-      <c r="Y64" s="17">
+      <c r="Y64" s="16">
         <v>0.25277234181343772</v>
       </c>
     </row>
@@ -50067,57 +49984,57 @@
       <c r="A68" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
-      <c r="I68" s="16"/>
-      <c r="J68" s="16">
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15">
         <v>0.30441400304414001</v>
       </c>
-      <c r="K68" s="16">
+      <c r="K68" s="15">
         <v>0.10147133434804669</v>
       </c>
-      <c r="L68" s="16">
+      <c r="L68" s="15">
         <v>0.40447488584474894</v>
       </c>
-      <c r="M68" s="16">
+      <c r="M68" s="15">
         <v>0.5811540058115402</v>
       </c>
-      <c r="N68" s="16">
+      <c r="N68" s="15">
         <v>0.53816046966731901</v>
       </c>
-      <c r="O68" s="16">
+      <c r="O68" s="15">
         <v>0.37067553048616708</v>
       </c>
-      <c r="P68" s="16">
+      <c r="P68" s="15">
         <v>0.57077625570776258</v>
       </c>
-      <c r="Q68" s="16">
+      <c r="Q68" s="15">
         <v>0.57500422797226458</v>
       </c>
-      <c r="R68" s="16">
+      <c r="R68" s="15">
         <v>0.70696146759593048</v>
       </c>
-      <c r="S68" s="16">
+      <c r="S68" s="15">
         <v>0.86924428402751963</v>
       </c>
-      <c r="T68" s="16">
+      <c r="T68" s="15">
         <v>2.5863099724480505</v>
       </c>
-      <c r="U68" s="16">
+      <c r="U68" s="15">
         <v>3.6549813955986812</v>
       </c>
-      <c r="V68" s="16">
+      <c r="V68" s="15">
         <v>4.036889720525596</v>
       </c>
-      <c r="W68" s="16">
+      <c r="W68" s="15">
         <v>6.2453375126974553</v>
       </c>
-      <c r="X68" s="16">
+      <c r="X68" s="15">
         <v>3.2548137163984849</v>
       </c>
     </row>
@@ -50125,73 +50042,73 @@
       <c r="A69" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="17">
+      <c r="B69" s="16">
         <v>0.17918731176527739</v>
       </c>
-      <c r="C69" s="17">
+      <c r="C69" s="16">
         <v>0.14535545467936098</v>
       </c>
-      <c r="D69" s="17">
+      <c r="D69" s="16">
         <v>0.15845780240593327</v>
       </c>
-      <c r="E69" s="17">
+      <c r="E69" s="16">
         <v>0.1498316039834055</v>
       </c>
-      <c r="F69" s="17">
+      <c r="F69" s="16">
         <v>0.1347902156764661</v>
       </c>
-      <c r="G69" s="17">
+      <c r="G69" s="16">
         <v>0.18958653994151151</v>
       </c>
-      <c r="H69" s="17">
+      <c r="H69" s="16">
         <v>0.18353719344825822</v>
       </c>
-      <c r="I69" s="17">
+      <c r="I69" s="16">
         <v>0.12836507928947488</v>
       </c>
-      <c r="J69" s="17">
+      <c r="J69" s="16">
         <v>0.12535509016122517</v>
       </c>
-      <c r="K69" s="17">
+      <c r="K69" s="16">
         <v>0.15416139825537606</v>
       </c>
-      <c r="L69" s="17">
+      <c r="L69" s="16">
         <v>0.21319901365069094</v>
       </c>
-      <c r="M69" s="17">
+      <c r="M69" s="16">
         <v>0.13556538436675425</v>
       </c>
-      <c r="N69" s="17">
+      <c r="N69" s="16">
         <v>0.1426745416205524</v>
       </c>
-      <c r="O69" s="17">
+      <c r="O69" s="16">
         <v>0.17089921406444017</v>
       </c>
-      <c r="P69" s="17">
+      <c r="P69" s="16">
         <v>0.18308207829936693</v>
       </c>
-      <c r="Q69" s="17">
+      <c r="Q69" s="16">
         <v>0.21797454043557021</v>
       </c>
-      <c r="R69" s="17">
+      <c r="R69" s="16">
         <v>0.16178813238750592</v>
       </c>
-      <c r="S69" s="17">
+      <c r="S69" s="16">
         <v>0.11826549026371555</v>
       </c>
-      <c r="T69" s="17">
+      <c r="T69" s="16">
         <v>0.18320015783762453</v>
       </c>
-      <c r="U69" s="17">
+      <c r="U69" s="16">
         <v>0.11430375923833559</v>
       </c>
-      <c r="V69" s="17">
+      <c r="V69" s="16">
         <v>0.11225524213694742</v>
       </c>
-      <c r="W69" s="17">
+      <c r="W69" s="16">
         <v>0.1716829439171017</v>
       </c>
-      <c r="X69" s="17">
+      <c r="X69" s="16">
         <v>0.13069358514235713</v>
       </c>
     </row>
@@ -50199,73 +50116,73 @@
       <c r="A70" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B70" s="16">
+      <c r="B70" s="15">
         <v>0.58751816400088952</v>
       </c>
-      <c r="C70" s="16">
+      <c r="C70" s="15">
         <v>0.63195855763612019</v>
       </c>
-      <c r="D70" s="16">
+      <c r="D70" s="15">
         <v>0.84807034848805107</v>
       </c>
-      <c r="E70" s="16">
+      <c r="E70" s="15">
         <v>0.72468873612271401</v>
       </c>
-      <c r="F70" s="16">
+      <c r="F70" s="15">
         <v>0.70518756353607848</v>
       </c>
-      <c r="G70" s="16">
+      <c r="G70" s="15">
         <v>0.78226961776024206</v>
       </c>
-      <c r="H70" s="16">
+      <c r="H70" s="15">
         <v>0.81749754243287398</v>
       </c>
-      <c r="I70" s="16">
+      <c r="I70" s="15">
         <v>0.88349648121868596</v>
       </c>
-      <c r="J70" s="16">
+      <c r="J70" s="15">
         <v>0.95119319991890894</v>
       </c>
-      <c r="K70" s="16">
+      <c r="K70" s="15">
         <v>0.92048229990249752</v>
       </c>
-      <c r="L70" s="16">
+      <c r="L70" s="15">
         <v>0.92005994960757642</v>
       </c>
-      <c r="M70" s="16">
+      <c r="M70" s="15">
         <v>0.98431753019201262</v>
       </c>
-      <c r="N70" s="16">
+      <c r="N70" s="15">
         <v>0.94540432280661413</v>
       </c>
-      <c r="O70" s="16">
+      <c r="O70" s="15">
         <v>0.81619276686525755</v>
       </c>
-      <c r="P70" s="16">
+      <c r="P70" s="15">
         <v>0.91711461765215874</v>
       </c>
-      <c r="Q70" s="16">
+      <c r="Q70" s="15">
         <v>0.88913935610658323</v>
       </c>
-      <c r="R70" s="16">
+      <c r="R70" s="15">
         <v>0.91556341739152636</v>
       </c>
-      <c r="S70" s="16">
+      <c r="S70" s="15">
         <v>0.90218624426321981</v>
       </c>
-      <c r="T70" s="16">
+      <c r="T70" s="15">
         <v>0.91672584775055033</v>
       </c>
-      <c r="U70" s="16">
+      <c r="U70" s="15">
         <v>0.942110199083116</v>
       </c>
-      <c r="V70" s="16">
+      <c r="V70" s="15">
         <v>0.94612082701666678</v>
       </c>
-      <c r="W70" s="16">
+      <c r="W70" s="15">
         <v>0.9382181082323805</v>
       </c>
-      <c r="X70" s="16">
+      <c r="X70" s="15">
         <v>0.93680249206717758</v>
       </c>
     </row>
@@ -50273,73 +50190,73 @@
       <c r="A71" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="B71" s="17">
+      <c r="B71" s="16">
         <v>1.3728687025740881E-2</v>
       </c>
-      <c r="C71" s="17">
+      <c r="C71" s="16">
         <v>8.9246408872480296E-3</v>
       </c>
-      <c r="D71" s="17">
+      <c r="D71" s="16">
         <v>1.4064542368890371E-2</v>
       </c>
-      <c r="E71" s="17">
+      <c r="E71" s="16">
         <v>1.3440969291696423E-2</v>
       </c>
-      <c r="F71" s="17">
+      <c r="F71" s="16">
         <v>1.4367639360976603E-2</v>
       </c>
-      <c r="G71" s="17">
+      <c r="G71" s="16">
         <v>1.06544901065449E-2</v>
       </c>
-      <c r="H71" s="17">
+      <c r="H71" s="16">
         <v>6.8721033906174785E-3</v>
       </c>
-      <c r="I71" s="17">
+      <c r="I71" s="16">
         <v>1.3383397499030053E-2</v>
       </c>
-      <c r="J71" s="17">
+      <c r="J71" s="16">
         <v>6.8134032678754683E-3</v>
       </c>
-      <c r="K71" s="17">
+      <c r="K71" s="16">
         <v>8.974387151398696E-3</v>
       </c>
-      <c r="L71" s="17">
+      <c r="L71" s="16">
         <v>1.0171012962918537E-2</v>
       </c>
-      <c r="M71" s="17">
+      <c r="M71" s="16">
         <v>4.0275281549390085E-3</v>
       </c>
-      <c r="N71" s="17">
+      <c r="N71" s="16">
         <v>5.4770281784942507E-3</v>
       </c>
-      <c r="O71" s="17">
+      <c r="O71" s="16">
         <v>5.9193423561722108E-3</v>
       </c>
-      <c r="P71" s="17">
+      <c r="P71" s="16">
         <v>5.7979529360833674E-3</v>
       </c>
-      <c r="Q71" s="17">
+      <c r="Q71" s="16">
         <v>5.9440758150922698E-3</v>
       </c>
-      <c r="R71" s="17">
+      <c r="R71" s="16">
         <v>1.0672682178439969E-2</v>
       </c>
-      <c r="S71" s="17">
+      <c r="S71" s="16">
         <v>1.3166338195431674E-2</v>
       </c>
-      <c r="T71" s="17">
+      <c r="T71" s="16">
         <v>1.0273264456408587E-2</v>
       </c>
-      <c r="U71" s="17">
+      <c r="U71" s="16">
         <v>1.1459284473580975E-2</v>
       </c>
-      <c r="V71" s="17">
+      <c r="V71" s="16">
         <v>1.0273784895450284E-2</v>
       </c>
-      <c r="W71" s="17">
+      <c r="W71" s="16">
         <v>1.1799059936493149E-2</v>
       </c>
-      <c r="X71" s="17">
+      <c r="X71" s="16">
         <v>1.5180712412366853E-2</v>
       </c>
     </row>
@@ -50347,59 +50264,59 @@
       <c r="A72" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
-      <c r="D72" s="16"/>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="16"/>
-      <c r="H72" s="16"/>
-      <c r="I72" s="16">
+      <c r="B72" s="15"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15">
         <v>0.22831050228310501</v>
       </c>
-      <c r="J72" s="16">
+      <c r="J72" s="15">
         <v>0.1906392694063927</v>
       </c>
-      <c r="K72" s="16">
+      <c r="K72" s="15">
         <v>0.18647260273972602</v>
       </c>
-      <c r="L72" s="16">
+      <c r="L72" s="15">
         <v>6.7876712328767116E-2</v>
       </c>
-      <c r="M72" s="16">
+      <c r="M72" s="15">
         <v>7.476575935480044E-2</v>
       </c>
-      <c r="N72" s="16">
+      <c r="N72" s="15">
         <v>9.6412405035707568E-2</v>
       </c>
-      <c r="O72" s="16">
+      <c r="O72" s="15">
         <v>0.15293804193529958</v>
       </c>
-      <c r="P72" s="16">
+      <c r="P72" s="15">
         <v>0.13941040865139273</v>
       </c>
-      <c r="Q72" s="16">
+      <c r="Q72" s="15">
         <v>0.1534278778672068</v>
       </c>
-      <c r="R72" s="16">
+      <c r="R72" s="15">
         <v>0.15383140488540142</v>
       </c>
-      <c r="S72" s="16">
+      <c r="S72" s="15">
         <v>0.15538589047072227</v>
       </c>
-      <c r="T72" s="16">
+      <c r="T72" s="15">
         <v>0.14838111835914639</v>
       </c>
-      <c r="U72" s="16">
+      <c r="U72" s="15">
         <v>0.15491400651998427</v>
       </c>
-      <c r="V72" s="16">
+      <c r="V72" s="15">
         <v>0.15239085998651261</v>
       </c>
-      <c r="W72" s="16">
+      <c r="W72" s="15">
         <v>0.13133926069138591</v>
       </c>
-      <c r="X72" s="16">
+      <c r="X72" s="15">
         <v>0.13764325363624622</v>
       </c>
     </row>
@@ -50407,65 +50324,65 @@
       <c r="A73" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B73" s="17"/>
-      <c r="C73" s="17"/>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
-      <c r="F73" s="17">
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16">
         <v>0.11415525114155251</v>
       </c>
-      <c r="G73" s="17">
+      <c r="G73" s="16">
         <v>6.5453767123287668E-2</v>
       </c>
-      <c r="H73" s="17">
+      <c r="H73" s="16">
         <v>8.4758159986470502E-2</v>
       </c>
-      <c r="I73" s="17">
+      <c r="I73" s="16">
         <v>0.17808980213089803</v>
       </c>
-      <c r="J73" s="17">
+      <c r="J73" s="16">
         <v>0.12192381639029079</v>
       </c>
-      <c r="K73" s="17">
+      <c r="K73" s="16">
         <v>8.1248714467892558E-2</v>
       </c>
-      <c r="L73" s="17">
+      <c r="L73" s="16">
         <v>0.15938903548169775</v>
       </c>
-      <c r="M73" s="17">
+      <c r="M73" s="16">
         <v>0.18169781142649755</v>
       </c>
-      <c r="N73" s="17">
+      <c r="N73" s="16">
         <v>0.2058669391554197</v>
       </c>
-      <c r="O73" s="17">
+      <c r="O73" s="16">
         <v>0.22956604290766625</v>
       </c>
-      <c r="P73" s="17">
+      <c r="P73" s="16">
         <v>0.2172995015710637</v>
       </c>
-      <c r="Q73" s="17">
+      <c r="Q73" s="16">
         <v>0.23704950320418605</v>
       </c>
-      <c r="R73" s="17">
+      <c r="R73" s="16">
         <v>0.23271503321770831</v>
       </c>
-      <c r="S73" s="17">
+      <c r="S73" s="16">
         <v>0.24584659524473154</v>
       </c>
-      <c r="T73" s="17">
+      <c r="T73" s="16">
         <v>0.21529025081619735</v>
       </c>
-      <c r="U73" s="17">
+      <c r="U73" s="16">
         <v>0.21381996798613462</v>
       </c>
-      <c r="V73" s="17">
+      <c r="V73" s="16">
         <v>0.23992922634315969</v>
       </c>
-      <c r="W73" s="17">
+      <c r="W73" s="16">
         <v>0.2323315222455867</v>
       </c>
-      <c r="X73" s="17">
+      <c r="X73" s="16">
         <v>0.24297964087912982</v>
       </c>
     </row>

</xml_diff>